<commit_message>
feat: Complete dashboard implementation with security hardening
-  Fix TeamMemberTabs data validation error by adding teamMembers array to /api/metrics/all endpoint
-  Replace all hardcoded Google Spreadsheet IDs with environment variables
-  Update .env.example files with comprehensive configuration templates
-  Add ENVIRONMENT_SETUP.md with detailed setup instructions
-  Implement proper CORS configuration and API connectivity
-  Add performance analytics and team management features
-  Ensure all sensitive credentials use environment variables only
-  Security: No sensitive data committed to repository
</commit_message>
<xml_diff>
--- a/finalyear-backend/logs/activity_log.xlsx
+++ b/finalyear-backend/logs/activity_log.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -450,9 +450,37 @@
         <v>Submitted metrics for 09/22/2025 - Assigned: 12, Resolved: 11, SLA Breaches: 1, Reopened: 10, Client Interactions: 12 | Remarks: N/A</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>10/17/2025, 03:18:09 PM</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Winnish Allwin G J</v>
+      </c>
+      <c r="C4" t="str">
+        <v>team_member</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Submitted metrics for 10/17/2025 - Assigned: 18, Resolved: 13, SLA Breaches: 2, Reopened: 1, Client Interactions: 13 | Remarks: N/A</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>10/17/2025, 03:29:42 PM</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Winnish Allwin G J</v>
+      </c>
+      <c r="C5" t="str">
+        <v>team_member</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Submitted metrics for 2025-10-17 - Assigned: 12, Resolved: 6, SLA Breaches: 1, Reopened: 3, Client Interactions: 5 | Remarks: N/A</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>